<commit_message>
draft bab 5 done
</commit_message>
<xml_diff>
--- a/Buku/Buku TA/Flow Ex.xlsx
+++ b/Buku/Buku TA/Flow Ex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sibobot\Buku\Buku TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97960606-5032-4064-834F-AB642543607A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446BAE5B-81D5-455D-A13D-DB3225C8AFA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{8806EF7A-5DBB-42D6-B5E0-D4EBF1B3B428}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{8806EF7A-5DBB-42D6-B5E0-D4EBF1B3B428}"/>
   </bookViews>
   <sheets>
     <sheet name="Pelanggan" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,10 @@
     <sheet name="Aspek Bisnis" sheetId="3" r:id="rId3"/>
     <sheet name="Rumus" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -51,9 +45,6 @@
     <t>RSUD Dr. Soetomo</t>
   </si>
   <si>
-    <t>Jl. Darmo 21 Surabaya</t>
-  </si>
-  <si>
     <t>Government</t>
   </si>
   <si>
@@ -199,6 +190,9 @@
   </si>
   <si>
     <t>MarginTg * 0.5 - RevenueTg * 0.1 - RevenueConTg * 0.1</t>
+  </si>
+  <si>
+    <t>Jl. Mayjen Prof. Dr. Moestopo No.6-8</t>
   </si>
 </sst>
 </file>
@@ -373,35 +367,35 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,7 +714,7 @@
   <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -758,7 +752,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -771,7 +765,7 @@
   <dimension ref="A2:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,95 +776,95 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2">
         <v>43561</v>
@@ -878,7 +872,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2">
         <v>43562</v>
@@ -886,7 +880,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2">
         <v>43563</v>
@@ -894,7 +888,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="9">
         <v>12</v>
@@ -910,7 +904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4D981A-6E5D-4299-B3FC-C333A91DCD24}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -928,134 +922,134 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="21"/>
+      <c r="F5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14" t="s">
+      <c r="G5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="14" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>32</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="20">
+      <c r="B12" s="18">
         <v>368520000</v>
       </c>
       <c r="C12" s="3">
@@ -1066,8 +1060,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="21"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="10">
         <v>0</v>
       </c>
@@ -1077,44 +1071,44 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="E15" s="21"/>
+      <c r="F15" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14" t="s">
+      <c r="G15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="14" t="s">
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="18">
+      <c r="A17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="16">
         <v>368520000</v>
       </c>
       <c r="C17" s="4"/>
@@ -1128,18 +1122,28 @@
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="19"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="A7:A8"/>
@@ -1150,16 +1154,6 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1170,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF85464-D33D-409B-8493-356A0A78EA72}">
   <dimension ref="A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1178,7 +1172,7 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>